<commit_message>
More work on grade reports.
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="102">
   <si>
     <r>
       <rPr>
@@ -40,6 +40,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2016-01-18</t>
     </r>
@@ -57,7 +58,7 @@
     <t xml:space="preserve">Klasse</t>
   </si>
   <si>
-    <t xml:space="preserve">12.Gym</t>
+    <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">Halbjahr</t>
@@ -277,9 +278,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">13</t>
@@ -403,6 +401,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -720,7 +719,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1109,44 +1108,44 @@
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="H9" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>82</v>
-      </c>
       <c r="I9" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="18" t="s">
-        <v>84</v>
-      </c>
       <c r="K9" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="O9" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
       <c r="S9" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="T9" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="V9" s="20" t="str">
         <f aca="false" t="array" ref="V9:V9">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(X9:AE9,"-",""),"+","")),"")),"00")</f>
@@ -1154,87 +1153,87 @@
       </c>
       <c r="X9" s="18"/>
       <c r="Y9" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z9" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA9" s="18"/>
       <c r="AB9" s="18"/>
       <c r="AC9" s="18"/>
       <c r="AD9" s="18"/>
       <c r="AE9" s="18" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="AF9" s="18"/>
       <c r="AH9" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AJ9" s="21" t="n">
         <f aca="false" t="array" ref="AJ9:AJ9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),1)</f>
         <v>10.7</v>
       </c>
       <c r="AK9" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AM9" s="22"/>
       <c r="AN9" s="22"/>
       <c r="AO9" s="22"/>
       <c r="AP9" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AQ9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="18" t="s">
+      <c r="H10" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="I10" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L10" s="18"/>
       <c r="M10" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="N10" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>93</v>
-      </c>
       <c r="O10" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
       <c r="S10" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T10" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V10" s="21" t="str">
         <f aca="false" t="array" ref="V10:V10">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O10:T10,"-",""),"+","")),"")),"00")</f>
@@ -1242,87 +1241,87 @@
       </c>
       <c r="X10" s="18"/>
       <c r="Y10" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z10" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
       <c r="AD10" s="18"/>
       <c r="AE10" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AF10" s="18"/>
       <c r="AH10" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AJ10" s="21" t="n">
         <f aca="false" t="array" ref="AJ10:AJ10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),1)</f>
         <v>7.5</v>
       </c>
       <c r="AK10" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AM10" s="22"/>
       <c r="AN10" s="22"/>
       <c r="AO10" s="22"/>
       <c r="AP10" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AQ10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="G11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="H11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>82</v>
-      </c>
       <c r="I11" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="O11" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T11" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V11" s="21" t="str">
         <f aca="false" t="array" ref="V11:V11">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O11:T11,"-",""),"+","")),"")),"00")</f>
@@ -1330,87 +1329,87 @@
       </c>
       <c r="X11" s="18"/>
       <c r="Y11" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z11" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA11" s="18"/>
       <c r="AB11" s="18"/>
       <c r="AC11" s="18"/>
       <c r="AD11" s="18"/>
       <c r="AE11" s="18" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="AF11" s="18"/>
       <c r="AH11" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AJ11" s="21" t="n">
         <f aca="false" t="array" ref="AJ11:AJ11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),1)</f>
         <v>11.3</v>
       </c>
       <c r="AK11" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AM11" s="22"/>
       <c r="AN11" s="22"/>
       <c r="AO11" s="22"/>
       <c r="AP11" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AQ11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L12" s="18"/>
       <c r="M12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="18"/>
       <c r="S12" s="18" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="T12" s="18" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="V12" s="21" t="str">
         <f aca="false" t="array" ref="V12:V12">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O12:T12,"-",""),"+","")),"")),"00")</f>
@@ -1418,87 +1417,87 @@
       </c>
       <c r="X12" s="18"/>
       <c r="Y12" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z12" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA12" s="18"/>
       <c r="AB12" s="18"/>
       <c r="AC12" s="18"/>
       <c r="AD12" s="18"/>
       <c r="AE12" s="18" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="AF12" s="18"/>
       <c r="AH12" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AJ12" s="21" t="n">
         <f aca="false" t="array" ref="AJ12:AJ12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),1)</f>
         <v>7.3</v>
       </c>
       <c r="AK12" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AM12" s="22"/>
       <c r="AN12" s="22"/>
       <c r="AO12" s="22"/>
       <c r="AP12" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AQ12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>101</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V13" s="21" t="str">
         <f aca="false" t="array" ref="V13:V13">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O13:T13,"-",""),"+","")),"")),"00")</f>
@@ -1506,34 +1505,34 @@
       </c>
       <c r="X13" s="18"/>
       <c r="Y13" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z13" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18"/>
       <c r="AE13" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AF13" s="18"/>
       <c r="AH13" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AJ13" s="21" t="n">
         <f aca="false" t="array" ref="AJ13:AJ13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),1)</f>
         <v>4.9</v>
       </c>
       <c r="AK13" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AM13" s="22"/>
       <c r="AN13" s="22"/>
       <c r="AO13" s="22"/>
       <c r="AP13" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AQ13" s="22"/>
     </row>

</xml_diff>

<commit_message>
Work on grade report template for Sek-II
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
   <si>
     <r>
       <rPr>
@@ -157,10 +157,7 @@
     <t xml:space="preserve">_DEM</t>
   </si>
   <si>
-    <t xml:space="preserve">_V12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_V13</t>
+    <t xml:space="preserve">_V_D</t>
   </si>
   <si>
     <t xml:space="preserve">_GS</t>
@@ -256,10 +253,7 @@
     <t xml:space="preserve">Φ De-En-Ma</t>
   </si>
   <si>
-    <t xml:space="preserve">Versetzung → Quali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versetzung → Quali 2</t>
+    <t xml:space="preserve">Versetzung → Quali 12/13</t>
   </si>
   <si>
     <t xml:space="preserve">Gleichstellungs-vermerk</t>
@@ -353,9 +347,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -542,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -630,6 +625,10 @@
     <xf numFmtId="165" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -712,14 +711,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AQ13"/>
+  <dimension ref="A1:AP13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="AC9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="AC1" activeCellId="0" sqref="AC1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="AM10" activeCellId="0" sqref="AM10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -739,8 +738,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="2.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="7.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="40" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="40" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -943,119 +943,113 @@
       <c r="AP6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AQ6" s="6" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
       <c r="E7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="O7" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="R7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="S7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="T7" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="U7" s="11"/>
       <c r="V7" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W7" s="11"/>
       <c r="X7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y7" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="Y7" s="10" t="s">
+      <c r="Z7" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="Z7" s="10" t="s">
+      <c r="AA7" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AA7" s="10" t="s">
+      <c r="AB7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AB7" s="10" t="s">
+      <c r="AC7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AC7" s="10" t="s">
+      <c r="AD7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AD7" s="10" t="s">
+      <c r="AE7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="AE7" s="10" t="s">
+      <c r="AF7" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="AF7" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="AG7" s="11"/>
       <c r="AH7" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI7" s="11"/>
       <c r="AJ7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK7" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="AK7" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="AL7" s="11"/>
       <c r="AM7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN7" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AN7" s="10" t="s">
+      <c r="AO7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AO7" s="10" t="s">
+      <c r="AP7" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="AP7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="AQ7" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1094,58 +1088,57 @@
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
-      <c r="AQ8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="18" t="s">
+      <c r="I9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="K9" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
       <c r="S9" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V9" s="20" t="str">
         <f aca="false" t="array" ref="V9:V9">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(X9:AE9,"-",""),"+","")),"")),"00")</f>
@@ -1153,10 +1146,10 @@
       </c>
       <c r="X9" s="18"/>
       <c r="Y9" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z9" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AA9" s="18"/>
       <c r="AB9" s="18"/>
@@ -1167,73 +1160,74 @@
       </c>
       <c r="AF9" s="18"/>
       <c r="AH9" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AJ9" s="21" t="n">
         <f aca="false" t="array" ref="AJ9:AJ9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),1)</f>
         <v>10.7</v>
       </c>
       <c r="AK9" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM9" s="22"/>
-      <c r="AN9" s="22"/>
-      <c r="AO9" s="22"/>
-      <c r="AP9" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ9" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="AM9" s="22" t="n">
+        <v>42535</v>
+      </c>
+      <c r="AN9" s="23"/>
+      <c r="AO9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="I10" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L10" s="18"/>
       <c r="M10" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
       <c r="S10" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T10" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V10" s="21" t="str">
         <f aca="false" t="array" ref="V10:V10">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O10:T10,"-",""),"+","")),"")),"00")</f>
@@ -1241,87 +1235,88 @@
       </c>
       <c r="X10" s="18"/>
       <c r="Y10" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z10" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
       <c r="AD10" s="18"/>
       <c r="AE10" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AF10" s="18"/>
       <c r="AH10" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AJ10" s="21" t="n">
         <f aca="false" t="array" ref="AJ10:AJ10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),1)</f>
         <v>7.5</v>
       </c>
       <c r="AK10" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM10" s="22"/>
-      <c r="AN10" s="22"/>
-      <c r="AO10" s="22"/>
-      <c r="AP10" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ10" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="AM10" s="22" t="n">
+        <v>42535</v>
+      </c>
+      <c r="AN10" s="23"/>
+      <c r="AO10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="I11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>84</v>
-      </c>
       <c r="K11" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="T11" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V11" s="21" t="str">
         <f aca="false" t="array" ref="V11:V11">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O11:T11,"-",""),"+","")),"")),"00")</f>
@@ -1329,10 +1324,10 @@
       </c>
       <c r="X11" s="18"/>
       <c r="Y11" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z11" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AA11" s="18"/>
       <c r="AB11" s="18"/>
@@ -1343,64 +1338,65 @@
       </c>
       <c r="AF11" s="18"/>
       <c r="AH11" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AJ11" s="21" t="n">
         <f aca="false" t="array" ref="AJ11:AJ11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),1)</f>
         <v>11.3</v>
       </c>
       <c r="AK11" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM11" s="22"/>
-      <c r="AN11" s="22"/>
-      <c r="AO11" s="22"/>
-      <c r="AP11" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ11" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="AM11" s="22" t="n">
+        <v>42535</v>
+      </c>
+      <c r="AN11" s="23"/>
+      <c r="AO11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="L12" s="18"/>
       <c r="M12" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
@@ -1417,10 +1413,10 @@
       </c>
       <c r="X12" s="18"/>
       <c r="Y12" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z12" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AA12" s="18"/>
       <c r="AB12" s="18"/>
@@ -1431,73 +1427,74 @@
       </c>
       <c r="AF12" s="18"/>
       <c r="AH12" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AJ12" s="21" t="n">
         <f aca="false" t="array" ref="AJ12:AJ12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),1)</f>
         <v>7.3</v>
       </c>
       <c r="AK12" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM12" s="22"/>
-      <c r="AN12" s="22"/>
-      <c r="AO12" s="22"/>
-      <c r="AP12" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ12" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="AM12" s="22" t="n">
+        <v>42535</v>
+      </c>
+      <c r="AN12" s="23"/>
+      <c r="AO12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="I13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="V13" s="21" t="str">
         <f aca="false" t="array" ref="V13:V13">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O13:T13,"-",""),"+","")),"")),"00")</f>
@@ -1505,65 +1502,61 @@
       </c>
       <c r="X13" s="18"/>
       <c r="Y13" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z13" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18"/>
       <c r="AE13" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AF13" s="18"/>
       <c r="AH13" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AJ13" s="21" t="n">
         <f aca="false" t="array" ref="AJ13:AJ13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),1)</f>
         <v>4.9</v>
       </c>
       <c r="AK13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM13" s="22"/>
-      <c r="AN13" s="22"/>
-      <c r="AO13" s="22"/>
-      <c r="AP13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ13" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="AM13" s="22" t="n">
+        <v>42535</v>
+      </c>
+      <c r="AN13" s="23"/>
+      <c r="AO13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP13" s="23"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="5">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:H13 J9:J13 L9:T9 V9:V13 X9:AF11 AH9:AH13 K10:T13 X12:X13 Z12:AF13" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ9:AK13 AP9:AP13" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ9:AK13 AO9:AO13" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AQ9:AQ13" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AP9:AP13" type="list">
       <formula1>"X,x"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM9:AM13" type="list">
-      <formula1>"Q"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AN9:AN13" type="list">
+      <formula1>"Erw,RS,HS"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AN9:AN13" type="list">
-      <formula1>"Q13,Erw,RS,HS"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AO9:AO13" type="list">
-      <formula1>"Erw,RS,HS"</formula1>
+    <dataValidation allowBlank="true" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM9:AM13" type="date">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Creation of grade entry tables (xlsx)
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Sp</t>
   </si>
   <si>
-    <t xml:space="preserve">_Ku</t>
+    <t xml:space="preserve">__Ku</t>
   </si>
   <si>
     <t xml:space="preserve">Bb</t>
@@ -151,10 +151,10 @@
     <t xml:space="preserve">Eu</t>
   </si>
   <si>
-    <t xml:space="preserve">_MITTEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_DEM</t>
+    <t xml:space="preserve">__AVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__DEM</t>
   </si>
   <si>
     <t xml:space="preserve">_V_D</t>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">Φ De-En-Ma</t>
   </si>
   <si>
-    <t xml:space="preserve">Versetzung → Quali 12/13</t>
+    <t xml:space="preserve">Versetzung (Quali)</t>
   </si>
   <si>
     <t xml:space="preserve">Gleichstellungs-vermerk</t>
@@ -711,14 +711,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AP13"/>
+  <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="AC9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="V9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AC1" activeCellId="0" sqref="AC1"/>
+      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AM10" activeCellId="0" sqref="AM10"/>
+      <selection pane="bottomRight" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -730,17 +730,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="5" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="2.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="24" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="29" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="40" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="28" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="39" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -778,7 +777,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="AJ2" s="5"/>
+      <c r="AI2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -895,52 +894,52 @@
       <c r="V6" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="W6" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="X6" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC6" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AH6" s="6" t="s">
+      <c r="AG6" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="AI6" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="AJ6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK6" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AL6" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="AM6" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AN6" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AO6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP6" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -999,56 +998,55 @@
       <c r="V7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="W7" s="11"/>
+      <c r="W7" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="X7" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Z7" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA7" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AC7" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AD7" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="10" t="s">
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AI7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AJ7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AL7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="AM7" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AN7" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AO7" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP7" s="10" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1074,6 +1072,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="V8" s="13"/>
+      <c r="W8" s="14"/>
       <c r="X8" s="14"/>
       <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
@@ -1082,12 +1081,11 @@
       <c r="AC8" s="14"/>
       <c r="AD8" s="14"/>
       <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
-      <c r="AH8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AL8" s="16"/>
       <c r="AM8" s="16"/>
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
-      <c r="AP8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
@@ -1141,42 +1139,42 @@
         <v>83</v>
       </c>
       <c r="V9" s="20" t="str">
-        <f aca="false" t="array" ref="V9:V9">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(X9:AE9,"-",""),"+","")),"")),"00")</f>
+        <f aca="false" t="array" ref="V9:V9">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W9:AD9,"-",""),"+","")),"")),"00")</f>
         <v>13</v>
       </c>
-      <c r="X9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="Y9" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z9" s="18" t="s">
         <v>83</v>
       </c>
+      <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
       <c r="AB9" s="18"/>
       <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="18" t="s">
+      <c r="AD9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="AF9" s="18"/>
-      <c r="AH9" s="18" t="s">
+      <c r="AE9" s="18"/>
+      <c r="AG9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AJ9" s="21" t="n">
-        <f aca="false" t="array" ref="AJ9:AJ9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),1)</f>
+      <c r="AI9" s="21" t="n">
+        <f aca="false" t="array" ref="AI9:AI9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),1)</f>
         <v>10.7</v>
       </c>
-      <c r="AK9" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM9" s="22" t="n">
+      <c r="AJ9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL9" s="22" t="n">
         <v>42535</v>
       </c>
-      <c r="AN9" s="23"/>
-      <c r="AO9" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP9" s="23"/>
+      <c r="AM9" s="23"/>
+      <c r="AN9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
@@ -1233,39 +1231,39 @@
         <f aca="false" t="array" ref="V10:V10">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O10:T10,"-",""),"+","")),"")),"00")</f>
         <v>12</v>
       </c>
-      <c r="X10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="Y10" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="Z10" s="18" t="s">
-        <v>82</v>
-      </c>
+      <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18" t="s">
+      <c r="AD10" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="AF10" s="18"/>
-      <c r="AH10" s="18" t="s">
+      <c r="AE10" s="18"/>
+      <c r="AG10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="AJ10" s="21" t="n">
-        <f aca="false" t="array" ref="AJ10:AJ10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),1)</f>
+      <c r="AI10" s="21" t="n">
+        <f aca="false" t="array" ref="AI10:AI10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),1)</f>
         <v>7.5</v>
       </c>
-      <c r="AK10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM10" s="22" t="n">
+      <c r="AJ10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL10" s="22" t="n">
         <v>42535</v>
       </c>
-      <c r="AN10" s="23"/>
-      <c r="AO10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
@@ -1322,39 +1320,39 @@
         <f aca="false" t="array" ref="V11:V11">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O11:T11,"-",""),"+","")),"")),"00")</f>
         <v>14</v>
       </c>
-      <c r="X11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="Y11" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z11" s="18" t="s">
         <v>83</v>
       </c>
+      <c r="Z11" s="18"/>
       <c r="AA11" s="18"/>
       <c r="AB11" s="18"/>
       <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18" t="s">
+      <c r="AD11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="AF11" s="18"/>
-      <c r="AH11" s="18" t="s">
+      <c r="AE11" s="18"/>
+      <c r="AG11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AJ11" s="21" t="n">
-        <f aca="false" t="array" ref="AJ11:AJ11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),1)</f>
+      <c r="AI11" s="21" t="n">
+        <f aca="false" t="array" ref="AI11:AI11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),1)</f>
         <v>11.3</v>
       </c>
-      <c r="AK11" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM11" s="22" t="n">
+      <c r="AJ11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL11" s="22" t="n">
         <v>42535</v>
       </c>
-      <c r="AN11" s="23"/>
-      <c r="AO11" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
@@ -1411,39 +1409,39 @@
         <f aca="false" t="array" ref="V12:V12">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O12:T12,"-",""),"+","")),"")),"00")</f>
         <v>12</v>
       </c>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z12" s="18" t="s">
+      <c r="W12" s="18"/>
+      <c r="X12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y12" s="18" t="s">
         <v>79</v>
       </c>
+      <c r="Z12" s="18"/>
       <c r="AA12" s="18"/>
       <c r="AB12" s="18"/>
       <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18" t="s">
+      <c r="AD12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="AF12" s="18"/>
-      <c r="AH12" s="18" t="s">
+      <c r="AE12" s="18"/>
+      <c r="AG12" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="AJ12" s="21" t="n">
-        <f aca="false" t="array" ref="AJ12:AJ12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),1)</f>
+      <c r="AI12" s="21" t="n">
+        <f aca="false" t="array" ref="AI12:AI12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),1)</f>
         <v>7.3</v>
       </c>
-      <c r="AK12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM12" s="22" t="n">
+      <c r="AJ12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL12" s="22" t="n">
         <v>42535</v>
       </c>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP12" s="23"/>
+      <c r="AM12" s="23"/>
+      <c r="AN12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
@@ -1500,62 +1498,62 @@
         <f aca="false" t="array" ref="V13:V13">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O13:T13,"-",""),"+","")),"")),"00")</f>
         <v>04</v>
       </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z13" s="18" t="s">
+      <c r="W13" s="18"/>
+      <c r="X13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y13" s="18" t="s">
         <v>79</v>
       </c>
+      <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18" t="s">
+      <c r="AD13" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="AF13" s="18"/>
-      <c r="AH13" s="18" t="s">
+      <c r="AE13" s="18"/>
+      <c r="AG13" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="AJ13" s="21" t="n">
-        <f aca="false" t="array" ref="AJ13:AJ13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),1)</f>
+      <c r="AI13" s="21" t="n">
+        <f aca="false" t="array" ref="AI13:AI13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),1)</f>
         <v>4.9</v>
       </c>
-      <c r="AK13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM13" s="22" t="n">
+      <c r="AJ13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL13" s="22" t="n">
         <v>42535</v>
       </c>
-      <c r="AN13" s="23"/>
-      <c r="AO13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP13" s="23"/>
+      <c r="AM13" s="23"/>
+      <c r="AN13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:H13 J9:J13 L9:T9 V9:V13 X9:AF11 AH9:AH13 K10:T13 X12:X13 Z12:AF13" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:H13 J9:J13 L9:T9 V9:AE11 AG9:AG13 K10:T13 V12:W13 Y12:AE13" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ9:AK13 AO9:AO13" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI9:AJ13 AN9:AN13" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AP9:AP13" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AO9:AO13" type="list">
       <formula1>"X,x"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AN9:AN13" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM9:AM13" type="list">
       <formula1>"Erw,RS,HS"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM9:AM13" type="date">
+    <dataValidation allowBlank="true" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL9:AL13" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Grade reports: more test data, tidying up, data.
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
@@ -13,37 +13,16 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Noten, Einsendeschluss </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2016-01-18</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
+  <si>
+    <t xml:space="preserve">Noten: Einsendeschluss 15.01.2016</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -88,9 +67,6 @@
     <t xml:space="preserve">Fr</t>
   </si>
   <si>
-    <t xml:space="preserve">AWT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bio</t>
   </si>
   <si>
@@ -103,69 +79,39 @@
     <t xml:space="preserve">Ges</t>
   </si>
   <si>
+    <t xml:space="preserve">Soz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mu</t>
   </si>
   <si>
-    <t xml:space="preserve">Ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soz</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sp</t>
   </si>
   <si>
     <t xml:space="preserve">__Ku</t>
   </si>
   <si>
-    <t xml:space="preserve">Bb</t>
-  </si>
-  <si>
     <t xml:space="preserve">FK</t>
   </si>
   <si>
     <t xml:space="preserve">Kge</t>
   </si>
   <si>
-    <t xml:space="preserve">Ktr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sth</t>
   </si>
   <si>
-    <t xml:space="preserve">Web</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eu</t>
   </si>
   <si>
     <t xml:space="preserve">__AVE</t>
   </si>
   <si>
-    <t xml:space="preserve">__DEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_V_D</t>
-  </si>
-  <si>
     <t xml:space="preserve">_GS</t>
   </si>
   <si>
-    <t xml:space="preserve">_Q12</t>
-  </si>
-  <si>
     <t xml:space="preserve">_BB</t>
   </si>
   <si>
@@ -184,9 +130,6 @@
     <t xml:space="preserve">Französisch</t>
   </si>
   <si>
-    <t xml:space="preserve">Arbeit-Wirtschaft-Technik</t>
-  </si>
-  <si>
     <t xml:space="preserve">Biologie</t>
   </si>
   <si>
@@ -199,69 +142,39 @@
     <t xml:space="preserve">Geschichte</t>
   </si>
   <si>
+    <t xml:space="preserve">Sozialkunde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Religion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Musik</t>
   </si>
   <si>
-    <t xml:space="preserve">Physik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Religion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sozialkunde</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sport</t>
   </si>
   <si>
     <t xml:space="preserve">Kunst</t>
   </si>
   <si>
-    <t xml:space="preserve">Buchbinden</t>
-  </si>
-  <si>
     <t xml:space="preserve">Freie Kunst</t>
   </si>
   <si>
     <t xml:space="preserve">Kunstgeschichte</t>
   </si>
   <si>
-    <t xml:space="preserve">Kupfertreiben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plastizieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schnitzen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Steinhauen</t>
   </si>
   <si>
-    <t xml:space="preserve">Weben</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eurythmie</t>
   </si>
   <si>
     <t xml:space="preserve">Φ Alle Fächer</t>
   </si>
   <si>
-    <t xml:space="preserve">Φ De-En-Ma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versetzung (Quali)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gleichstellungs-vermerk</t>
   </si>
   <si>
-    <t xml:space="preserve">Abschluss 12.Kl.</t>
-  </si>
-  <si>
     <t xml:space="preserve">„Blauer Brief“</t>
   </si>
   <si>
@@ -283,10 +196,10 @@
     <t xml:space="preserve">11</t>
   </si>
   <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
     <t xml:space="preserve">/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05</t>
   </si>
   <si>
     <t xml:space="preserve">nt</t>
@@ -352,7 +265,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -391,14 +304,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -421,7 +326,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,7 +336,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF777777"/>
-        <bgColor rgb="FF888888"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8FFB4"/>
+        <bgColor rgb="FFDDE8CB"/>
       </patternFill>
     </fill>
     <fill>
@@ -455,25 +366,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBF819E"/>
-        <bgColor rgb="FF888888"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
         <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC8FFB4"/>
-        <bgColor rgb="FFDDE8CB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF888888"/>
-        <bgColor rgb="FF777777"/>
       </patternFill>
     </fill>
     <fill>
@@ -537,12 +436,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,19 +453,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -570,15 +469,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -586,12 +485,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -602,35 +497,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -660,7 +555,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF888888"/>
+      <rgbColor rgb="FF777777"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFDDE8CB"/>
@@ -691,7 +586,7 @@
       <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF4000"/>
-      <rgbColor rgb="FF777777"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -711,50 +606,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AO13"/>
+  <dimension ref="A1:AM1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="V9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="AL1" activeCellId="0" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="5" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="28" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="39" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="1.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="13" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="19" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9.38"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="26" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="28" style="1" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="1" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="37" style="1" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="38" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -780,10 +684,10 @@
       <c r="AI2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -808,10 +712,10 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -859,195 +763,147 @@
       <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="6"/>
       <c r="Q6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="V6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="W6" s="6"/>
+      <c r="X6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="Y6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="X6" s="6" t="s">
+      <c r="AE6" s="6"/>
+      <c r="AG6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="AI6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AM6" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
       <c r="E7" s="10" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>47</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P7" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="Q7" s="10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>56</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
       <c r="U7" s="11"/>
       <c r="V7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="W7" s="10" t="s">
-        <v>58</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="W7" s="10"/>
       <c r="X7" s="10" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z7" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB7" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC7" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
       <c r="AD7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE7" s="10" t="s">
-        <v>66</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="AE7" s="10"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="10" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="AH7" s="11"/>
       <c r="AI7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ7" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK7" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="10"/>
       <c r="AL7" s="10" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="AM7" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN7" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO7" s="10" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1082,72 +938,69 @@
       <c r="AD8" s="14"/>
       <c r="AE8" s="14"/>
       <c r="AG8" s="15"/>
+      <c r="AK8" s="16"/>
       <c r="AL8" s="16"/>
       <c r="AM8" s="16"/>
-      <c r="AN8" s="16"/>
-      <c r="AO8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>80</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I9" s="18"/>
       <c r="J9" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>80</v>
+        <v>58</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="T9" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="V9" s="20" t="str">
-        <f aca="false" t="array" ref="V9:V9">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W9:AD9,"-",""),"+","")),"")),"00")</f>
+      <c r="Q9" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="V9" s="19" t="str">
+        <f aca="false" t="array" ref="V9:V9">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W9:AE9,"-",""),"+","")),"")),"0")</f>
         <v>13</v>
       </c>
       <c r="W9" s="18"/>
       <c r="X9" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="Y9" s="18" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
@@ -1158,174 +1011,154 @@
       </c>
       <c r="AE9" s="18"/>
       <c r="AG9" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI9" s="21" t="n">
-        <f aca="false" t="array" ref="AI9:AI9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),1)</f>
-        <v>10.7</v>
-      </c>
-      <c r="AJ9" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL9" s="22" t="n">
-        <v>42535</v>
-      </c>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO9" s="23"/>
+        <v>61</v>
+      </c>
+      <c r="AI9" s="20" t="n">
+        <f aca="false" t="array" ref="AI9:AI9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),2)</f>
+        <v>10.67</v>
+      </c>
+      <c r="AK9" s="21"/>
+      <c r="AL9" s="22"/>
+      <c r="AM9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="18" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>80</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="I10" s="18"/>
       <c r="J10" s="18" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="L10" s="18"/>
       <c r="M10" s="18" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T10" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="V10" s="21" t="str">
-        <f aca="false" t="array" ref="V10:V10">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O10:T10,"-",""),"+","")),"")),"00")</f>
-        <v>12</v>
+      <c r="Q10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="V10" s="19" t="e">
+        <f aca="false" t="array" ref="V10:V10">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W10:AE10,"-",""),"+","")),"")),"0")</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="W10" s="18"/>
       <c r="X10" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="Y10" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
       <c r="AD10" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="AE10" s="18"/>
       <c r="AG10" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI10" s="21" t="n">
-        <f aca="false" t="array" ref="AI10:AI10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),1)</f>
-        <v>7.5</v>
-      </c>
-      <c r="AJ10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL10" s="22" t="n">
-        <v>42535</v>
-      </c>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO10" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="AI10" s="20" t="n">
+        <f aca="false" t="array" ref="AI10:AI10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),2)</f>
+        <v>7.09</v>
+      </c>
+      <c r="AK10" s="21"/>
+      <c r="AL10" s="22"/>
+      <c r="AM10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>80</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I11" s="18"/>
       <c r="J11" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="T11" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="V11" s="21" t="str">
-        <f aca="false" t="array" ref="V11:V11">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O11:T11,"-",""),"+","")),"")),"00")</f>
-        <v>14</v>
+      <c r="Q11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="V11" s="19" t="str">
+        <f aca="false" t="array" ref="V11:V11">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W11:AE11,"-",""),"+","")),"")),"0")</f>
+        <v>13</v>
       </c>
       <c r="W11" s="18"/>
       <c r="X11" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="Y11" s="18" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="Z11" s="18"/>
       <c r="AA11" s="18"/>
@@ -1336,85 +1169,75 @@
       </c>
       <c r="AE11" s="18"/>
       <c r="AG11" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI11" s="21" t="n">
-        <f aca="false" t="array" ref="AI11:AI11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),1)</f>
-        <v>11.3</v>
-      </c>
-      <c r="AJ11" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL11" s="22" t="n">
-        <v>42535</v>
-      </c>
-      <c r="AM11" s="23"/>
-      <c r="AN11" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO11" s="23"/>
+        <v>61</v>
+      </c>
+      <c r="AI11" s="20" t="n">
+        <f aca="false" t="array" ref="AI11:AI11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),2)</f>
+        <v>11.2</v>
+      </c>
+      <c r="AK11" s="21"/>
+      <c r="AL11" s="22"/>
+      <c r="AM11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="18" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>80</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="I12" s="18"/>
       <c r="J12" s="18" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="L12" s="18"/>
       <c r="M12" s="18" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18" t="s">
+      <c r="Q12" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="T12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="V12" s="21" t="str">
-        <f aca="false" t="array" ref="V12:V12">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O12:T12,"-",""),"+","")),"")),"00")</f>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="V12" s="19" t="str">
+        <f aca="false" t="array" ref="V12:V12">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W12:AE12,"-",""),"+","")),"")),"0")</f>
         <v>12</v>
       </c>
       <c r="W12" s="18"/>
-      <c r="X12" s="19" t="s">
-        <v>80</v>
+      <c r="X12" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="Y12" s="18" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="Z12" s="18"/>
       <c r="AA12" s="18"/>
@@ -1425,141 +1248,171 @@
       </c>
       <c r="AE12" s="18"/>
       <c r="AG12" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI12" s="21" t="n">
-        <f aca="false" t="array" ref="AI12:AI12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),1)</f>
+        <v>57</v>
+      </c>
+      <c r="AI12" s="20" t="n">
+        <f aca="false" t="array" ref="AI12:AI12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),2)</f>
         <v>7.3</v>
       </c>
-      <c r="AJ12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL12" s="22" t="n">
-        <v>42535</v>
-      </c>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO12" s="23"/>
+      <c r="AK12" s="21"/>
+      <c r="AL12" s="22"/>
+      <c r="AM12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="18" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>80</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="I13" s="18"/>
       <c r="J13" s="18" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="V13" s="21" t="str">
-        <f aca="false" t="array" ref="V13:V13">TEXT( AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(O13:T13,"-",""),"+","")),"")),"00")</f>
-        <v>04</v>
+      <c r="Q13" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="V13" s="19" t="str">
+        <f aca="false" t="array" ref="V13:V13">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W13:AE13,"-",""),"+","")),"")),"0")</f>
+        <v>6</v>
       </c>
       <c r="W13" s="18"/>
-      <c r="X13" s="19" t="s">
-        <v>80</v>
+      <c r="X13" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="Y13" s="18" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="AE13" s="18"/>
       <c r="AG13" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI13" s="21" t="n">
-        <f aca="false" t="array" ref="AI13:AI13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),1)</f>
-        <v>4.9</v>
-      </c>
-      <c r="AJ13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL13" s="22" t="n">
-        <v>42535</v>
-      </c>
-      <c r="AM13" s="23"/>
-      <c r="AN13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO13" s="23"/>
+        <v>57</v>
+      </c>
+      <c r="AI13" s="20" t="n">
+        <f aca="false" t="array" ref="AI13:AI13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),2)</f>
+        <v>5.1</v>
+      </c>
+      <c r="AK13" s="21"/>
+      <c r="AL13" s="22"/>
+      <c r="AM13" s="22"/>
     </row>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:H13 J9:J13 L9:T9 V9:AE11 AG9:AG13 K10:T13 V12:W13 Y12:AE13" type="list">
+  <dataValidations count="6">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V9:V13" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI9:AI13" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM9:AM13" type="list">
+      <formula1>"X,x"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AK9:AK13" type="date">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:T13 W9:AE13 AG9:AG13" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI9:AJ13 AN9:AN13" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AO9:AO13" type="list">
-      <formula1>"X,x"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM9:AM13" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL9:AL13" type="list">
       <formula1>"Erw,RS,HS"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL9:AL13" type="date">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.636805555555555" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
More work on grade reports and grade tables.
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Noten_1/Notentabelle_12-Gym.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
   <si>
     <t xml:space="preserve">Noten: Einsendeschluss 15.01.2016</t>
   </si>
@@ -91,6 +91,9 @@
     <t xml:space="preserve">Sp</t>
   </si>
   <si>
+    <t xml:space="preserve">AWT</t>
+  </si>
+  <si>
     <t xml:space="preserve">__Ku</t>
   </si>
   <si>
@@ -152,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbeit-Wirtschaft-Technik</t>
   </si>
   <si>
     <t xml:space="preserve">Kunst</t>
@@ -326,7 +332,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +383,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFDEDCE6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
         <bgColor rgb="FFDEDCE6"/>
       </patternFill>
@@ -436,7 +448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,7 +525,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,11 +533,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -554,7 +570,7 @@
       <rgbColor rgb="FFB47804"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF777777"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -613,7 +629,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AL1" activeCellId="0" sqref="AL1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,7 +643,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="1" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="13" style="1" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="19" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="2.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="1" width="7.49"/>
@@ -790,120 +807,124 @@
         <v>22</v>
       </c>
       <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
+      <c r="T6" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="V6" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W6" s="6"/>
       <c r="X6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE6" s="6"/>
       <c r="AG6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AK6" s="6"/>
       <c r="AL6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AM6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
       <c r="E7" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
+      <c r="T7" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="U7" s="11"/>
       <c r="V7" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="W7" s="10"/>
       <c r="X7" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
       <c r="AD7" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AH7" s="11"/>
       <c r="AI7" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AJ7" s="11"/>
       <c r="AK7" s="10"/>
       <c r="AL7" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AM7" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -944,63 +965,67 @@
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="P9" s="18"/>
+        <v>62</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="Q9" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" s="18"/>
+      <c r="T9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="V9" s="19" t="str">
-        <f aca="false" t="array" ref="V9:V9">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W9:AE9,"-",""),"+","")),"")),"0")</f>
+      <c r="V9" s="20" t="str">
+        <f aca="false" t="array" ref="V9:V9">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W9:AE9,"-",""),"+","")),"")),"00"),"*")</f>
         <v>13</v>
       </c>
       <c r="W9" s="18"/>
       <c r="X9" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Y9" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
@@ -1011,154 +1036,162 @@
       </c>
       <c r="AE9" s="18"/>
       <c r="AG9" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI9" s="20" t="n">
+        <v>63</v>
+      </c>
+      <c r="AI9" s="21" t="n">
         <f aca="false" t="array" ref="AI9:AI9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),2)</f>
         <v>10.67</v>
       </c>
-      <c r="AK9" s="21"/>
-      <c r="AL9" s="22"/>
-      <c r="AM9" s="22"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="23"/>
+      <c r="AM9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L10" s="18"/>
       <c r="M10" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="P10" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="Q10" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R10" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S10" s="18"/>
+      <c r="T10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="V10" s="19" t="e">
-        <f aca="false" t="array" ref="V10:V10">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W10:AE10,"-",""),"+","")),"")),"0")</f>
-        <v>#DIV/0!</v>
+      <c r="V10" s="20" t="str">
+        <f aca="false" t="array" ref="V10:V10">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W10:AE10,"-",""),"+","")),"")),"00"),"*")</f>
+        <v>*</v>
       </c>
       <c r="W10" s="18"/>
       <c r="X10" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Y10" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
       <c r="AD10" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE10" s="18"/>
       <c r="AG10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI10" s="20" t="n">
+        <v>57</v>
+      </c>
+      <c r="AI10" s="21" t="n">
         <f aca="false" t="array" ref="AI10:AI10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),2)</f>
         <v>7.09</v>
       </c>
-      <c r="AK10" s="21"/>
-      <c r="AL10" s="22"/>
-      <c r="AM10" s="22"/>
+      <c r="AK10" s="22"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="P11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="P11" s="18"/>
       <c r="Q11" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S11" s="18"/>
+      <c r="T11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="V11" s="19" t="str">
-        <f aca="false" t="array" ref="V11:V11">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W11:AE11,"-",""),"+","")),"")),"0")</f>
+      <c r="V11" s="20" t="str">
+        <f aca="false" t="array" ref="V11:V11">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W11:AE11,"-",""),"+","")),"")),"00"),"*")</f>
         <v>13</v>
       </c>
       <c r="W11" s="18"/>
       <c r="X11" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Y11" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Z11" s="18"/>
       <c r="AA11" s="18"/>
@@ -1169,75 +1202,79 @@
       </c>
       <c r="AE11" s="18"/>
       <c r="AG11" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI11" s="20" t="n">
+        <v>63</v>
+      </c>
+      <c r="AI11" s="21" t="n">
         <f aca="false" t="array" ref="AI11:AI11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),2)</f>
         <v>11.2</v>
       </c>
-      <c r="AK11" s="21"/>
-      <c r="AL11" s="22"/>
-      <c r="AM11" s="22"/>
+      <c r="AK11" s="22"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L12" s="18"/>
       <c r="M12" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="P12" s="18"/>
+      <c r="P12" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="Q12" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R12" s="18" t="s">
         <v>5</v>
       </c>
       <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="V12" s="19" t="str">
-        <f aca="false" t="array" ref="V12:V12">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W12:AE12,"-",""),"+","")),"")),"0")</f>
+      <c r="T12" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="V12" s="20" t="str">
+        <f aca="false" t="array" ref="V12:V12">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W12:AE12,"-",""),"+","")),"")),"00"),"*")</f>
         <v>12</v>
       </c>
       <c r="W12" s="18"/>
       <c r="X12" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y12" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="Y12" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="Z12" s="18"/>
       <c r="AA12" s="18"/>
@@ -1248,94 +1285,98 @@
       </c>
       <c r="AE12" s="18"/>
       <c r="AG12" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI12" s="20" t="n">
+        <v>59</v>
+      </c>
+      <c r="AI12" s="21" t="n">
         <f aca="false" t="array" ref="AI12:AI12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),2)</f>
         <v>7.3</v>
       </c>
-      <c r="AK12" s="21"/>
-      <c r="AL12" s="22"/>
-      <c r="AM12" s="22"/>
+      <c r="AK12" s="22"/>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>66</v>
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P13" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="P13" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="Q13" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="V13" s="19" t="str">
-        <f aca="false" t="array" ref="V13:V13">TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W13:AE13,"-",""),"+","")),"")),"0")</f>
-        <v>6</v>
+      <c r="T13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="V13" s="20" t="str">
+        <f aca="false" t="array" ref="V13:V13">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W13:AE13,"-",""),"+","")),"")),"00"),"*")</f>
+        <v>06</v>
       </c>
       <c r="W13" s="18"/>
       <c r="X13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y13" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="Y13" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AE13" s="18"/>
       <c r="AG13" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI13" s="20" t="n">
+        <v>59</v>
+      </c>
+      <c r="AI13" s="21" t="n">
         <f aca="false" t="array" ref="AI13:AI13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),2)</f>
         <v>5.1</v>
       </c>
-      <c r="AK13" s="21"/>
-      <c r="AL13" s="22"/>
-      <c r="AM13" s="22"/>
+      <c r="AK13" s="22"/>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="23"/>
     </row>
     <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1385,7 +1426,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V9:V13" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -1402,12 +1443,16 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:T13 W9:AE13 AG9:AG13" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:S13 W9:AE13 AG9:AG13" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL9:AL13" type="list">
       <formula1>"Erw,RS,HS"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T9:T13" type="none">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>